<commit_message>
Correcciones y nuevas variables para base final
</commit_message>
<xml_diff>
--- a/data/otras/refcode.xlsx
+++ b/data/otras/refcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diplomado CSC\proyecto-china\data\otras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C1B643-8783-4D8C-9CD8-1AA6442C7B59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7A01B7-188A-4931-A953-192B20F3A681}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1530,8 +1530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>